<commit_message>
Updated Sample Data Excel File
</commit_message>
<xml_diff>
--- a/pythonUpdate/SampleInput.xlsx
+++ b/pythonUpdate/SampleInput.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\SRUCourseScheduling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\SRUCourseScheduling\pythonUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283325CF-B2F8-4CB0-B728-3564376C2379}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786F334C-C27D-4113-BC5D-367DAAEC76C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5875EC4F-3BA3-4AFB-A351-DABC9B9C1EBA}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Teacher</t>
   </si>
@@ -46,15 +46,6 @@
     <t>Classes Not Available</t>
   </si>
   <si>
-    <t>MATH 273, STAT 102</t>
-  </si>
-  <si>
-    <t>8-9, 10-11</t>
-  </si>
-  <si>
-    <t>9-10, 10-11</t>
-  </si>
-  <si>
     <t>Class</t>
   </si>
   <si>
@@ -119,6 +110,27 @@
   </si>
   <si>
     <t>Num_Sections</t>
+  </si>
+  <si>
+    <t>8,9,10</t>
+  </si>
+  <si>
+    <t>9,10</t>
+  </si>
+  <si>
+    <t>Hurl</t>
+  </si>
+  <si>
+    <t>MATH 313, STAT 102</t>
+  </si>
+  <si>
+    <t>STAT 102</t>
+  </si>
+  <si>
+    <t>12,3,4</t>
+  </si>
+  <si>
+    <t>930,2</t>
   </si>
 </sst>
 </file>
@@ -470,10 +482,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E5A8AE-C5F4-4C02-BA03-5684F580691D}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -489,19 +501,19 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
@@ -509,22 +521,36 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>4</v>
+        <v>25</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F2">
         <v>6</v>
       </c>
       <c r="G2">
         <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
@@ -534,10 +560,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E900E0F6-1D7B-4274-A6B9-E990F5B64F38}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -547,38 +573,38 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
         <v>24</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -586,7 +612,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -594,9 +620,17 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6">
         <v>3</v>
       </c>
     </row>
@@ -622,33 +656,33 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Completed handleTime function that converts columns of numerical series into the corresponding encoded time arrays
</commit_message>
<xml_diff>
--- a/pythonUpdate/SampleInput.xlsx
+++ b/pythonUpdate/SampleInput.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\SRUCourseScheduling\pythonUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{786F334C-C27D-4113-BC5D-367DAAEC76C0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6497C8F3-95D9-4C7A-8ED9-E1A5F6BAB5CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5875EC4F-3BA3-4AFB-A351-DABC9B9C1EBA}"/>
   </bookViews>
@@ -130,7 +130,7 @@
     <t>12,3,4</t>
   </si>
   <si>
-    <t>930,2</t>
+    <t>9,2</t>
   </si>
 </sst>
 </file>
@@ -485,7 +485,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Began working on handling classes in an OO fashion
</commit_message>
<xml_diff>
--- a/pythonUpdate/SampleInput.xlsx
+++ b/pythonUpdate/SampleInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\SRUCourseScheduling\pythonUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6497C8F3-95D9-4C7A-8ED9-E1A5F6BAB5CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E85878-43D6-4C4F-8B18-A8B64587123A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5875EC4F-3BA3-4AFB-A351-DABC9B9C1EBA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="18240" windowHeight="29040" activeTab="1" xr2:uid="{5875EC4F-3BA3-4AFB-A351-DABC9B9C1EBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Teacher" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>Teacher</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>9,2</t>
+  </si>
+  <si>
+    <t>MATH 401, MATH 125</t>
   </si>
 </sst>
 </file>
@@ -484,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E5A8AE-C5F4-4C02-BA03-5684F580691D}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,8 +565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E900E0F6-1D7B-4274-A6B9-E990F5B64F38}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -599,7 +602,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>32</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -609,6 +615,9 @@
       <c r="B3">
         <v>1</v>
       </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -617,6 +626,9 @@
       <c r="B4">
         <v>4</v>
       </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
@@ -625,6 +637,12 @@
       <c r="B5">
         <v>3</v>
       </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -632,6 +650,9 @@
       </c>
       <c r="B6">
         <v>3</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Somehow i think i finished?
</commit_message>
<xml_diff>
--- a/pythonUpdate/SampleInput.xlsx
+++ b/pythonUpdate/SampleInput.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\SRUCourseScheduling\pythonUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B35659-134E-4EDE-BCA0-54810FFEABDB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8AB947-577E-42E4-9DF3-6DCD85557DB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12960" windowWidth="18240" windowHeight="29040" activeTab="1" xr2:uid="{5875EC4F-3BA3-4AFB-A351-DABC9B9C1EBA}"/>
+    <workbookView xWindow="28680" yWindow="-12960" windowWidth="18240" windowHeight="29040" xr2:uid="{5875EC4F-3BA3-4AFB-A351-DABC9B9C1EBA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Teacher" sheetId="1" r:id="rId1"/>
+    <sheet name="Prof" sheetId="1" r:id="rId1"/>
     <sheet name="Classes" sheetId="2" r:id="rId2"/>
     <sheet name="Rooms" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>Teacher</t>
   </si>
@@ -43,9 +43,6 @@
     <t>Marchard</t>
   </si>
   <si>
-    <t>Classes Not Available</t>
-  </si>
-  <si>
     <t>Class</t>
   </si>
   <si>
@@ -82,12 +79,6 @@
     <t>BML 201</t>
   </si>
   <si>
-    <t>MWF Room-Time Exceptions</t>
-  </si>
-  <si>
-    <t>TTh Room-Time Exceptions</t>
-  </si>
-  <si>
     <t>Min Credits</t>
   </si>
   <si>
@@ -118,21 +109,12 @@
     <t>Hurl</t>
   </si>
   <si>
-    <t>MATH 313, STAT 102</t>
-  </si>
-  <si>
     <t>STAT 102</t>
   </si>
   <si>
     <t>12,3,4</t>
   </si>
   <si>
-    <t>9,2</t>
-  </si>
-  <si>
-    <t>MATH 401, MATH 125</t>
-  </si>
-  <si>
     <t>Room_Exceptions</t>
   </si>
   <si>
@@ -152,6 +134,27 @@
   </si>
   <si>
     <t>TTh_Room-Time_Exceptions</t>
+  </si>
+  <si>
+    <t>MATH 401,MATH 125</t>
+  </si>
+  <si>
+    <t>MATH 313,STAT 102</t>
+  </si>
+  <si>
+    <t>1,2,3</t>
+  </si>
+  <si>
+    <t>VSC 201,VSC 203</t>
+  </si>
+  <si>
+    <t>VSC 201,VSC 202</t>
+  </si>
+  <si>
+    <t>Required_Course</t>
+  </si>
+  <si>
+    <t>Non_Course</t>
   </si>
 </sst>
 </file>
@@ -503,10 +506,94 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E5A8AE-C5F4-4C02-BA03-5684F580691D}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:H3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="5" width="15.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2">
+        <v>6</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3">
+        <v>6</v>
+      </c>
+      <c r="H3">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E900E0F6-1D7B-4274-A6B9-E990F5B64F38}">
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,135 +603,57 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>32</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="G1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G2">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2">
-        <v>6</v>
-      </c>
-      <c r="G2">
-        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E900E0F6-1D7B-4274-A6B9-E990F5B64F38}">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="5" width="15.6328125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-      <c r="F1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
         <v>5</v>
-      </c>
-      <c r="B2">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E2" t="s">
-        <v>35</v>
-      </c>
-      <c r="G2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>6</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="D3" t="s">
-        <v>37</v>
-      </c>
       <c r="E3">
         <v>10</v>
       </c>
@@ -654,16 +663,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="E4" t="s">
-        <v>36</v>
+        <v>30</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -671,19 +683,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E5" t="s">
         <v>28</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
       </c>
       <c r="G5">
         <v>1</v>
@@ -691,16 +703,19 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B6">
         <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E6">
         <v>3</v>
+      </c>
+      <c r="F6" t="s">
+        <v>13</v>
       </c>
       <c r="G6">
         <v>2</v>
@@ -716,7 +731,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,33 +743,54 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C1" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added inclusion of all input variables to be passed to matlab
</commit_message>
<xml_diff>
--- a/pythonUpdate/SampleInput.xlsx
+++ b/pythonUpdate/SampleInput.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Documents\SRUCourseScheduling\pythonUpdate\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8AB947-577E-42E4-9DF3-6DCD85557DB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10EBE68C-6AE0-4021-B4EA-1E4FB22F073F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-12960" windowWidth="18240" windowHeight="29040" xr2:uid="{5875EC4F-3BA3-4AFB-A351-DABC9B9C1EBA}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{5875EC4F-3BA3-4AFB-A351-DABC9B9C1EBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Prof" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="41">
   <si>
     <t>Teacher</t>
   </si>
@@ -155,6 +155,9 @@
   </si>
   <si>
     <t>Non_Course</t>
+  </si>
+  <si>
+    <t>Max Preps</t>
   </si>
 </sst>
 </file>
@@ -506,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E5A8AE-C5F4-4C02-BA03-5684F580691D}">
-  <dimension ref="A1:H3"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -517,7 +520,7 @@
     <col min="1" max="5" width="15.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -542,8 +545,11 @@
       <c r="H1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -565,8 +571,11 @@
       <c r="H2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -581,6 +590,9 @@
       </c>
       <c r="H3">
         <v>12</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>